<commit_message>
jpeg data model generation in Graphiz + copy in markdown img folder
</commit_message>
<xml_diff>
--- a/data_selection/data_selection.xlsx
+++ b/data_selection/data_selection.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="228">
   <si>
     <t xml:space="preserve">source_gv</t>
   </si>
@@ -241,6 +241,9 @@
     <t xml:space="preserve">[validFrom]</t>
   </si>
   <si>
+    <t xml:space="preserve">Date ouverture POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">R</t>
   </si>
   <si>
@@ -250,6 +253,9 @@
     <t xml:space="preserve">[validThrough]</t>
   </si>
   <si>
+    <t xml:space="preserve">Date fermeture POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
@@ -259,6 +265,9 @@
     <t xml:space="preserve">[hasContact]</t>
   </si>
   <si>
+    <t xml:space="preserve">Contact POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">T</t>
   </si>
   <si>
@@ -268,6 +277,9 @@
     <t xml:space="preserve">[homepage]</t>
   </si>
   <si>
+    <t xml:space="preserve">Site internet POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">U</t>
   </si>
   <si>
@@ -277,6 +289,9 @@
     <t xml:space="preserve">[email]</t>
   </si>
   <si>
+    <t xml:space="preserve">email POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">V</t>
   </si>
   <si>
@@ -286,6 +301,9 @@
     <t xml:space="preserve">[telephone]</t>
   </si>
   <si>
+    <t xml:space="preserve">Telephone POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">W</t>
   </si>
   <si>
@@ -295,6 +313,9 @@
     <t xml:space="preserve">[offers]</t>
   </si>
   <si>
+    <t xml:space="preserve">Condition tarifaire</t>
+  </si>
+  <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
@@ -304,6 +325,9 @@
     <t xml:space="preserve">[priceSpecification]</t>
   </si>
   <si>
+    <t xml:space="preserve">Specification tarifaire</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
@@ -313,6 +337,9 @@
     <t xml:space="preserve">[minPrice]</t>
   </si>
   <si>
+    <t xml:space="preserve">prix minimum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Z</t>
   </si>
   <si>
@@ -322,6 +349,9 @@
     <t xml:space="preserve">[maxPrice]</t>
   </si>
   <si>
+    <t xml:space="preserve">prix maximum</t>
+  </si>
+  <si>
     <t xml:space="preserve">AA</t>
   </si>
   <si>
@@ -340,6 +370,9 @@
     <t xml:space="preserve">[topObjectProperty]</t>
   </si>
   <si>
+    <t xml:space="preserve">Propriete du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AC</t>
   </si>
   <si>
@@ -349,6 +382,9 @@
     <t xml:space="preserve">[shortDescription]</t>
   </si>
   <si>
+    <t xml:space="preserve">Courte description POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AD</t>
   </si>
   <si>
@@ -358,6 +394,9 @@
     <t xml:space="preserve">[asTheme]</t>
   </si>
   <si>
+    <t xml:space="preserve">Theme du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AE</t>
   </si>
   <si>
@@ -379,6 +418,9 @@
     <t xml:space="preserve">[hasReviewValue]</t>
   </si>
   <si>
+    <t xml:space="preserve">Note du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AG</t>
   </si>
   <si>
@@ -388,6 +430,9 @@
     <t xml:space="preserve">[Tour]</t>
   </si>
   <si>
+    <t xml:space="preserve">Itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AH</t>
   </si>
   <si>
@@ -397,6 +442,9 @@
     <t xml:space="preserve">[TourType]</t>
   </si>
   <si>
+    <t xml:space="preserve">Type d’itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AI</t>
   </si>
   <si>
@@ -406,6 +454,9 @@
     <t xml:space="preserve">[TourPath]</t>
   </si>
   <si>
+    <t xml:space="preserve">Etape de l’itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AJ</t>
   </si>
   <si>
@@ -415,6 +466,9 @@
     <t xml:space="preserve">[elevation]</t>
   </si>
   <si>
+    <t xml:space="preserve">denivelé de l’itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AK</t>
   </si>
   <si>
@@ -442,6 +496,9 @@
     <t xml:space="preserve">[durantionDays]</t>
   </si>
   <si>
+    <t xml:space="preserve">Duree en jour de l’itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AN</t>
   </si>
   <si>
@@ -451,6 +508,9 @@
     <t xml:space="preserve">[arrivedAt]</t>
   </si>
   <si>
+    <t xml:space="preserve">Lieu de destination de l’itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AO</t>
   </si>
   <si>
@@ -460,6 +520,9 @@
     <t xml:space="preserve">[tourDistance]</t>
   </si>
   <si>
+    <t xml:space="preserve">Distance en metre de l’itineraire</t>
+  </si>
+  <si>
     <t xml:space="preserve">AP</t>
   </si>
   <si>
@@ -469,6 +532,9 @@
     <t xml:space="preserve">[hasAudience]</t>
   </si>
   <si>
+    <t xml:space="preserve">clientèle cible du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AQ</t>
   </si>
   <si>
@@ -478,6 +544,9 @@
     <t xml:space="preserve">[requiredMaxAge]</t>
   </si>
   <si>
+    <t xml:space="preserve">age max du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AR</t>
   </si>
   <si>
@@ -487,6 +556,9 @@
     <t xml:space="preserve">[requiredMinAge]</t>
   </si>
   <si>
+    <t xml:space="preserve">age min du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AS</t>
   </si>
   <si>
@@ -496,6 +568,9 @@
     <t xml:space="preserve">[requiredGender]</t>
   </si>
   <si>
+    <t xml:space="preserve">sexe exige du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AT</t>
   </si>
   <si>
@@ -505,6 +580,9 @@
     <t xml:space="preserve">[hasFeature]</t>
   </si>
   <si>
+    <t xml:space="preserve">equipement du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AU</t>
   </si>
   <si>
@@ -514,6 +592,9 @@
     <t xml:space="preserve">[occupancy]</t>
   </si>
   <si>
+    <t xml:space="preserve">capacite en nombre de personnes du POI</t>
+  </si>
+  <si>
     <t xml:space="preserve">AV</t>
   </si>
   <si>
@@ -521,6 +602,9 @@
   </si>
   <si>
     <t xml:space="preserve">[numberOf Rooms]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre de chambre du POI</t>
   </si>
   <si>
     <t xml:space="preserve">Iness</t>
@@ -891,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F49" activeCellId="0" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1267,23 +1351,29 @@
       <c r="E18" s="4" t="s">
         <v>71</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A18),4,1),(ROW(A18)&gt;26)+1)</f>
         <v>R</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,71 +1381,83 @@
         <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C20" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A19),4,1),(ROW(A19)&gt;26)+1)</f>
         <v>S</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C21" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A20),4,1),(ROW(A20)&gt;26)+1)</f>
         <v>T</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C22" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A21),4,1),(ROW(A21)&gt;26)+1)</f>
         <v>U</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C23" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A22),4,1),(ROW(A22)&gt;26)+1)</f>
         <v>V</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,89 +1465,104 @@
         <v>8</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C24" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A23),4,1),(ROW(A23)&gt;26)+1)</f>
         <v>W</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C25" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A24),4,1),(ROW(A24)&gt;26)+1)</f>
         <v>X</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>92</v>
+        <v>99</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C26" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A25),4,1),(ROW(A25)&gt;26)+1)</f>
         <v>Y</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>95</v>
+        <v>103</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C27" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A26),4,1),(ROW(A26)&gt;26)+1)</f>
         <v>Z</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>98</v>
+        <v>107</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C28" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A27),4,1),(ROW(A27)&gt;26)+1)</f>
         <v>AA</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>101</v>
+        <v>111</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,35 +1570,41 @@
         <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C29" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A28),4,1),(ROW(A28)&gt;26)+1)</f>
         <v>AB</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>104</v>
+        <v>114</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C30" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A29),4,1),(ROW(A29)&gt;26)+1)</f>
         <v>AC</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>107</v>
+        <v>118</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,17 +1612,20 @@
         <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C31" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A30),4,1),(ROW(A30)&gt;26)+1)</f>
         <v>AD</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>110</v>
+        <v>122</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,38 +1633,41 @@
         <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C32" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A31),4,1),(ROW(A31)&gt;26)+1)</f>
         <v>AE</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C33" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A32),4,1),(ROW(A32)&gt;26)+1)</f>
         <v>AF</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,164 +1675,188 @@
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C34" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A33),4,1),(ROW(A33)&gt;26)+1)</f>
         <v>AG</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>120</v>
+        <v>134</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C35" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A34),4,1),(ROW(A34)&gt;26)+1)</f>
         <v>AH</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>123</v>
+        <v>138</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C36" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A35),4,1),(ROW(A35)&gt;26)+1)</f>
         <v>AI</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>126</v>
+        <v>142</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="C37" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A36),4,1),(ROW(A36)&gt;26)+1)</f>
         <v>AJ</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="6"/>
+        <v>146</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="C38" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A37),4,1),(ROW(A37)&gt;26)+1)</f>
         <v>AK</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F38" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="C39" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A38),4,1),(ROW(A38)&gt;26)+1)</f>
         <v>AL</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C40" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A39),4,1),(ROW(A39)&gt;26)+1)</f>
         <v>AM</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>138</v>
+        <v>156</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C41" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A40),4,1),(ROW(A40)&gt;26)+1)</f>
         <v>AN</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>141</v>
+        <v>160</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C42" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A41),4,1),(ROW(A41)&gt;26)+1)</f>
         <v>AO</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>144</v>
+        <v>164</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,71 +1864,83 @@
         <v>8</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C43" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A42),4,1),(ROW(A42)&gt;26)+1)</f>
         <v>AP</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>147</v>
+        <v>168</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="C44" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A43),4,1),(ROW(A43)&gt;26)+1)</f>
         <v>AQ</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="C45" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A44),4,1),(ROW(A44)&gt;26)+1)</f>
         <v>AR</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="C46" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A45),4,1),(ROW(A45)&gt;26)+1)</f>
         <v>AS</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>156</v>
+        <v>180</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1783,53 +1948,62 @@
         <v>8</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C47" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A46),4,1),(ROW(A46)&gt;26)+1)</f>
         <v>AT</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>159</v>
+        <v>184</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="C48" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A47),4,1),(ROW(A47)&gt;26)+1)</f>
         <v>AU</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>162</v>
+        <v>188</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="C49" s="0" t="str">
         <f aca="false">LEFT(ADDRESS(1,ROW(A48),4,1),(ROW(A48)&gt;26)+1)</f>
         <v>AV</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>165</v>
+        <v>192</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,117 +2047,117 @@
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2015,7 +2189,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="313.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2044,18 +2218,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2063,60 +2237,60 @@
         <v>18</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>